<commit_message>
add: profiles, example. extensions, valueset 4 zib-FeedingPatternInfant
</commit_message>
<xml_diff>
--- a/Mappings/FeedingPatternInfant - STU3.xlsx
+++ b/Mappings/FeedingPatternInfant - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="11970" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="180">
   <si>
     <t>Subject</t>
   </si>
@@ -566,12 +566,21 @@
     <t>.component.feedingType extension where 
 • extension zib-FeedingPatternInfant-FeedingMethod =  http://nictiz.nl/fhir/StructureDefinition/extension-feedingpatterninfant-feedingmethod</t>
   </si>
+  <si>
+    <t>SNOMED CT:373453009 | Nutritional supplement (substance)</t>
+  </si>
+  <si>
+    <t>SNOMED CT: 289145007 |Finding of infant feeding pattern (finding)</t>
+  </si>
+  <si>
+    <t>280987003 | Food and drink type (qualifier value) |</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -613,6 +622,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -710,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -777,6 +792,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -991,7 +1015,7 @@
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="635000" y="635000"/>
+    <xdr:pos x="667844" y="720397"/>
     <xdr:ext cx="6010275" cy="4419600"/>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1009,7 +1033,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="667844" y="720397"/>
           <a:ext cx="6010275" cy="4419600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2886,7 +2910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
@@ -3688,10 +3712,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S11"/>
+  <dimension ref="B2:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3754,7 +3778,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="25.5">
+    <row r="3" spans="2:19" ht="51">
       <c r="B3" s="9" t="s">
         <v>68</v>
       </c>
@@ -3777,7 +3801,9 @@
       <c r="M3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="25" t="s">
+        <v>178</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
         <v>165</v>
@@ -3800,7 +3826,7 @@
       <c r="H4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="22" t="s">
         <v>75</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -3826,16 +3852,16 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="2:19" ht="25.5">
+    <row r="5" spans="2:19" ht="38.25">
       <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="26" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="22" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3847,13 +3873,15 @@
       <c r="K5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="25" t="s">
+        <v>177</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
         <v>169</v>
@@ -3864,14 +3892,14 @@
     </row>
     <row r="6" spans="2:19" ht="38.25">
       <c r="B6" s="12"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="26" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="22" t="s">
         <v>87</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -3883,13 +3911,13 @@
       <c r="K6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="22" t="s">
         <v>91</v>
       </c>
       <c r="O6" s="2"/>
@@ -3924,7 +3952,7 @@
       <c r="L7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="22" t="s">
         <v>95</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -3976,7 +4004,7 @@
     </row>
     <row r="9" spans="2:19" ht="114.75">
       <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="27" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="16"/>
@@ -4081,6 +4109,11 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="2"/>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="M13" s="25" t="s">
+        <v>179</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4100,7 +4133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -4189,7 +4224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>

</xml_diff>